<commit_message>
'discount_group field returned because it is necessary'
</commit_message>
<xml_diff>
--- a/files/cp.xlsx
+++ b/files/cp.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Пользовательская корзина, пересчитано: 2021-02-05 17:14</t>
+          <t>Пользовательская корзина, пересчитано: 2021-02-13 21:16</t>
         </is>
       </c>
     </row>
@@ -583,12 +583,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>003G1006</t>
+          <t>003G1018</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AFD 0.05..0.35</t>
+          <t>AFP 0.05..0.35</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>1317.15</v>
+        <v>1518.66</v>
       </c>
       <c r="G8">
         <f>$C$4</f>
@@ -626,7 +626,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">AF </t>
+          <t>AF</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>45.46</v>
@@ -659,27 +659,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>065B2388</t>
+          <t>065B3050</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>VFG2 15/4.0</t>
+          <t>VFM2 15/0.25</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>28RU PL08-IWKB</t>
+          <t>40RU PL08-DH-V</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>733.4400000000001</v>
+        <v>353.43</v>
       </c>
       <c r="G10">
-        <f>$C$4</f>
+        <f>$C$3</f>
         <v/>
       </c>
       <c r="H10">
@@ -697,27 +697,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>003G1006</t>
+          <t>082G6007</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>AFD 0.05..0.35</t>
+          <t>ARV152/230/pulse</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>28RU PL08-IWKB</t>
+          <t>40RU PL08-DH-V</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1317.15</v>
+        <v>564.01</v>
       </c>
       <c r="G11">
-        <f>$C$4</f>
+        <f>$C$3</f>
         <v/>
       </c>
       <c r="H11">
@@ -730,483 +730,27 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>6</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>003G1391</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AF </t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="n">
-        <v>45.46</v>
-      </c>
-      <c r="G12">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H12">
-        <f>ROUND(F12*((100-G12)/100)*E12, 2)</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>ROUND(H12*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>7</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>065B3052</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>VFM2 15/0.63</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>40RU PL08-DH-V</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="n">
-        <v>353.43</v>
-      </c>
-      <c r="G13">
-        <f>$C$3</f>
-        <v/>
-      </c>
-      <c r="H13">
-        <f>ROUND(F13*((100-G13)/100)*E13, 2)</f>
-        <v/>
-      </c>
-      <c r="I13">
-        <f>ROUND(H13*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>082G6007</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ARV152/230/pulse</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>40RU PL08-DH-V</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>564.01</v>
-      </c>
-      <c r="G14">
-        <f>$C$3</f>
-        <v/>
-      </c>
-      <c r="H14">
-        <f>ROUND(F14*((100-G14)/100)*E14, 2)</f>
-        <v/>
-      </c>
-      <c r="I14">
-        <f>ROUND(H14*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>9</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>065B2390</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>VFG2 25/8.0</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>842.14</v>
-      </c>
-      <c r="G15">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H15">
-        <f>ROUND(F15*((100-G15)/100)*E15, 2)</f>
-        <v/>
-      </c>
-      <c r="I15">
-        <f>ROUND(H15*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>10</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>003G1017</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>AFP 0.1..0.7</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1012.42</v>
-      </c>
-      <c r="G16">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H16">
-        <f>ROUND(F16*((100-G16)/100)*E16, 2)</f>
-        <v/>
-      </c>
-      <c r="I16">
-        <f>ROUND(H16*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>11</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>003G1391</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AF </t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>2</v>
-      </c>
-      <c r="F17" t="n">
-        <v>45.46</v>
-      </c>
-      <c r="G17">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H17">
-        <f>ROUND(F17*((100-G17)/100)*E17, 2)</f>
-        <v/>
-      </c>
-      <c r="I17">
-        <f>ROUND(H17*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>12</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>065B2388</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>VFG2 15/4.0</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" t="n">
-        <v>733.4400000000001</v>
-      </c>
-      <c r="G18">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H18">
-        <f>ROUND(F18*((100-G18)/100)*E18, 2)</f>
-        <v/>
-      </c>
-      <c r="I18">
-        <f>ROUND(H18*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>13</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>003G1013</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>AFA 0.05..0.35</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1620.23</v>
-      </c>
-      <c r="G19">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H19">
-        <f>ROUND(F19*((100-G19)/100)*E19, 2)</f>
-        <v/>
-      </c>
-      <c r="I19">
-        <f>ROUND(H19*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>14</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>003G1391</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AF </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" t="n">
-        <v>45.46</v>
-      </c>
-      <c r="G20">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H20">
-        <f>ROUND(F20*((100-G20)/100)*E20, 2)</f>
-        <v/>
-      </c>
-      <c r="I20">
-        <f>ROUND(H20*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>15</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>065B2388</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>VFG2 15/4.0</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="n">
-        <v>733.4400000000001</v>
-      </c>
-      <c r="G21">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H21">
-        <f>ROUND(F21*((100-G21)/100)*E21, 2)</f>
-        <v/>
-      </c>
-      <c r="I21">
-        <f>ROUND(H21*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>16</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>003G1013</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>AFA 0.05..0.35</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1620.23</v>
-      </c>
-      <c r="G22">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H22">
-        <f>ROUND(F22*((100-G22)/100)*E22, 2)</f>
-        <v/>
-      </c>
-      <c r="I22">
-        <f>ROUND(H22*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>17</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>003G1391</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AF </t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>28RU PL08-IWKB</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="n">
-        <v>45.46</v>
-      </c>
-      <c r="G23">
-        <f>$C$4</f>
-        <v/>
-      </c>
-      <c r="H23">
-        <f>ROUND(F23*((100-G23)/100)*E23, 2)</f>
-        <v/>
-      </c>
-      <c r="I23">
-        <f>ROUND(H23*120%, 2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="D24" s="2" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>Общее кол-во:</t>
         </is>
       </c>
-      <c r="E24" s="2">
-        <f>SUBTOTAL(9, E7:E23)</f>
-        <v/>
-      </c>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="2" t="inlineStr">
+      <c r="E12" s="2">
+        <f>SUBTOTAL(9, E7:E11)</f>
+        <v/>
+      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>Итого:</t>
         </is>
       </c>
-      <c r="H24" s="2">
-        <f>SUBTOTAL(9, H7:H23)</f>
-        <v/>
-      </c>
-      <c r="I24" s="2">
-        <f>SUBTOTAL(9, I7:I23)</f>
+      <c r="H12" s="2">
+        <f>SUBTOTAL(9, H7:H11)</f>
+        <v/>
+      </c>
+      <c r="I12" s="2">
+        <f>SUBTOTAL(9, I7:I11)</f>
         <v/>
       </c>
     </row>

</xml_diff>